<commit_message>
Highlighter and report added
</commit_message>
<xml_diff>
--- a/identifyCourse/Output/Output.xlsx
+++ b/identifyCourse/Output/Output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2809" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2809" uniqueCount="103">
   <si>
     <t>COURSE NAME</t>
   </si>
@@ -49,73 +49,73 @@
     <t>English</t>
   </si>
   <si>
-    <t>1238</t>
+    <t>1239</t>
   </si>
   <si>
     <t>Russian</t>
   </si>
   <si>
-    <t>630</t>
+    <t>624</t>
   </si>
   <si>
     <t>Spanish</t>
   </si>
   <si>
-    <t>620</t>
+    <t>614</t>
   </si>
   <si>
     <t>French</t>
   </si>
   <si>
-    <t>583</t>
+    <t>577</t>
   </si>
   <si>
     <t>Portuguese (Portugal)</t>
   </si>
   <si>
-    <t>541</t>
+    <t>536</t>
   </si>
   <si>
     <t>Arabic</t>
   </si>
   <si>
-    <t>483</t>
+    <t>480</t>
   </si>
   <si>
     <t>Vietnamese</t>
   </si>
   <si>
-    <t>475</t>
+    <t>473</t>
   </si>
   <si>
     <t>German</t>
   </si>
   <si>
-    <t>474</t>
+    <t>472</t>
   </si>
   <si>
     <t>Italian</t>
   </si>
   <si>
-    <t>457</t>
+    <t>455</t>
   </si>
   <si>
     <t>Chinese (China)</t>
   </si>
   <si>
-    <t>137</t>
+    <t>136</t>
   </si>
   <si>
     <t>Korean</t>
   </si>
   <si>
-    <t>127</t>
+    <t>126</t>
   </si>
   <si>
     <t>Portuguese (Brazil)</t>
   </si>
   <si>
-    <t>68</t>
+    <t>69</t>
   </si>
   <si>
     <t>Turkish</t>
@@ -172,10 +172,13 @@
     <t>12</t>
   </si>
   <si>
+    <t>Urdu</t>
+  </si>
+  <si>
     <t>Portuguese</t>
   </si>
   <si>
-    <t>Urdu</t>
+    <t>11</t>
   </si>
   <si>
     <t>Dutch</t>
@@ -286,7 +289,7 @@
     <t>TOTAL COURSES</t>
   </si>
   <si>
-    <t>11745</t>
+    <t>11681</t>
   </si>
   <si>
     <t>LEVEL NAME</t>
@@ -298,28 +301,28 @@
     <t>Intermediate</t>
   </si>
   <si>
-    <t>592</t>
+    <t>594</t>
   </si>
   <si>
     <t>Beginner</t>
   </si>
   <si>
-    <t>581</t>
+    <t>584</t>
   </si>
   <si>
     <t>Mixed</t>
   </si>
   <si>
-    <t>159</t>
+    <t>155</t>
   </si>
   <si>
     <t>Advanced</t>
   </si>
   <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>1391</t>
+    <t>60</t>
+  </si>
+  <si>
+    <t>1393</t>
   </si>
 </sst>
 </file>
@@ -614,231 +617,231 @@
         <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
         <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
         <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
         <v>69</v>
-      </c>
-      <c r="B36" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
         <v>75</v>
-      </c>
-      <c r="B40" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
         <v>81</v>
-      </c>
-      <c r="B45" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" t="s">
         <v>85</v>
-      </c>
-      <c r="B48" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -860,50 +863,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>